<commit_message>
Made a project part 1 folder.
</commit_message>
<xml_diff>
--- a/Project Part 1/Proj1_control_signals.xlsx
+++ b/Project Part 1/Proj1_control_signals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishakn\Research\CPRE3810\Project\Proj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC381E14-8BD6-49EA-A8EF-AF8CAE9B3D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C691369-9EC6-4E52-87A6-16D75D897DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00D6E995-B1C9-9941-8016-EE5CE3EB0628}"/>
   </bookViews>
@@ -180,22 +180,22 @@
     </r>
   </si>
   <si>
-    <t>ImmSrc</t>
-  </si>
-  <si>
-    <r>
-      <t>1 [</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>addi should sign extend immediate</t>
+    <t>ImmType</t>
+  </si>
+  <si>
+    <r>
+      <t>000 [</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I-type sign extend 12 (instruction[31-20]) bits to 32 bits</t>
     </r>
     <r>
       <rPr>
@@ -581,10 +581,10 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
     <col min="3" max="3" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="51.625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27" style="1" bestFit="1" customWidth="1"/>

</xml_diff>